<commit_message>
Hopefullu to teleuteo commit
</commit_message>
<xml_diff>
--- a/WebGames/App_Data/omades_scores.xlsx
+++ b/WebGames/App_Data/omades_scores.xlsx
@@ -176,35 +176,6 @@
         <charset val="161"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="15"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="161"/>
-        <scheme val="minor"/>
-      </font>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -283,6 +254,35 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="161"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -297,14 +297,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B50" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B50" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="3" tableBorderDxfId="4" totalsRowBorderDxfId="2">
   <autoFilter ref="A1:B50"/>
   <sortState ref="A2:B50">
     <sortCondition descending="1" ref="B1:B50"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="Ομάδα" dataDxfId="2"/>
-    <tableColumn id="2" name="Σκορ" dataDxfId="1"/>
+    <tableColumn id="1" name="Ομάδα" dataDxfId="1"/>
+    <tableColumn id="2" name="Σκορ" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -610,14 +610,15 @@
   <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="28.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -633,7 +634,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="3">
-        <v>33270</v>
+        <v>34870</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -649,7 +650,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="3">
-        <v>32168</v>
+        <v>32568</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -686,90 +687,90 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3">
-        <v>29004</v>
+        <v>29282</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="B10" s="3">
-        <v>28497</v>
+        <v>29044</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B11" s="3">
-        <v>28223</v>
+        <v>29004</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="B12" s="3">
-        <v>27929</v>
+        <v>28741</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B13" s="3">
-        <v>27777</v>
+        <v>28562</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B14" s="3">
-        <v>27319</v>
+        <v>28497</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="B15" s="3">
-        <v>27282</v>
+        <v>28254</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="B16" s="3">
-        <v>27254</v>
+        <v>28223</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="B17" s="3">
-        <v>27162</v>
+        <v>28129</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B18" s="3">
-        <v>27044</v>
+        <v>28055</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B19" s="3">
-        <v>26941</v>
+        <v>27777</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -777,23 +778,23 @@
         <v>24</v>
       </c>
       <c r="B20" s="3">
-        <v>26762</v>
+        <v>27562</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="B21" s="3">
-        <v>26757</v>
+        <v>27319</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B22" s="3">
-        <v>26458</v>
+        <v>27106</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -801,127 +802,127 @@
         <v>1</v>
       </c>
       <c r="B23" s="3">
-        <v>26453</v>
+        <v>27053</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B24" s="3">
-        <v>26313</v>
+        <v>26757</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B25" s="3">
-        <v>25255</v>
+        <v>26713</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="B26" s="3">
-        <v>25134</v>
+        <v>26458</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B27" s="3">
-        <v>25125</v>
+        <v>25938</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B28" s="3">
-        <v>25106</v>
+        <v>25370</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B29" s="3">
-        <v>24970</v>
+        <v>25134</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B30" s="3">
-        <v>24083</v>
+        <v>25125</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B31" s="3">
-        <v>23768</v>
+        <v>24483</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="B32" s="3">
-        <v>23720</v>
+        <v>24368</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B33" s="3">
-        <v>23683</v>
+        <v>23964</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="B34" s="3">
-        <v>23538</v>
+        <v>23920</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B35" s="3">
-        <v>23485</v>
+        <v>23683</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B36" s="3">
-        <v>23284</v>
+        <v>23485</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B37" s="3">
-        <v>22737</v>
+        <v>23284</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B38" s="3">
-        <v>22564</v>
+        <v>22737</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -937,63 +938,63 @@
         <v>9</v>
       </c>
       <c r="B40" s="3">
-        <v>21960</v>
+        <v>22160</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B41" s="3">
-        <v>21528</v>
+        <v>21568</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B42" s="3">
-        <v>21462</v>
+        <v>21528</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B43" s="3">
-        <v>21205</v>
+        <v>21508</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B44" s="3">
-        <v>20708</v>
+        <v>21462</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="B45" s="3">
-        <v>20543</v>
+        <v>21205</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="B46" s="3">
-        <v>20411</v>
+        <v>20543</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="B47" s="3">
-        <v>20368</v>
+        <v>20411</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>